<commit_message>
small changes to model and graphs in excel file
</commit_message>
<xml_diff>
--- a/docs/Randomness in code explained.xlsx
+++ b/docs/Randomness in code explained.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>Default</t>
   </si>
@@ -129,6 +129,24 @@
   </si>
   <si>
     <t>job5_Modifier</t>
+  </si>
+  <si>
+    <t>fractionHouseholdsInCity</t>
+  </si>
+  <si>
+    <t>Job attractiveness</t>
+  </si>
+  <si>
+    <t>fractionPeopleInService</t>
+  </si>
+  <si>
+    <t>Job 3 attractiveness</t>
+  </si>
+  <si>
+    <t>fractionPeopleInNonProfit</t>
+  </si>
+  <si>
+    <t>Job 6 attractiveness</t>
   </si>
 </sst>
 </file>
@@ -207,7 +225,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -441,11 +458,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="48385408"/>
-        <c:axId val="48383872"/>
+        <c:axId val="133758976"/>
+        <c:axId val="133760512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48385408"/>
+        <c:axId val="133758976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -455,12 +472,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48383872"/>
+        <c:crossAx val="133760512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48383872"/>
+        <c:axId val="133760512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,7 +488,582 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48385408"/>
+        <c:crossAx val="133758976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Job 1 and 2 attractiveness</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>JobXAttractiveness!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Job attractiveness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>JobXAttractiveness!$H$2:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>JobXAttractiveness!$I$2:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.32500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.27500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="66419328"/>
+        <c:axId val="66417792"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="66419328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66417792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="66417792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="66419328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>JobXAttractiveness!$I$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Job 3 attractiveness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>JobXAttractiveness!$H$15:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>JobXAttractiveness!$I$15:$I$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44117647058823534</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36764705882352944</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.29411764705882354</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22058823529411764</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1470588235294118</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.3529411764705843E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="71716224"/>
+        <c:axId val="71714688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="71716224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71714688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="71714688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71716224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>JobXAttractiveness!$I$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Job 6 attractiveness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>JobXAttractiveness!$H$51:$H$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>JobXAttractiveness!$I$51:$I$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70588235294117641</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55882352941176472</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45454545454545447</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.37878787878787873</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30303030303030298</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22727272727272718</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.15151515151515138</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.575757575757569E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.1102230246251565E-16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="70268032"/>
+        <c:axId val="69905792"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="70268032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69905792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="69905792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70268032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -520,6 +1112,101 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1241,10 +1928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,14 +1941,22 @@
     <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1274,8 +1969,15 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>IF(H2&lt;(0.4/5),1-(0.5 / (0.4/5))*H2,0.5-0.5*H2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1291,13 +1993,36 @@
       <c r="E3">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I12" si="0">IF(H3&lt;(0.4/5),1-(0.5 / (0.4/5))*H3,0.5-0.5*H3)</f>
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -1310,8 +2035,15 @@
       <c r="E6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1327,262 +2059,540 @@
       <c r="E7">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="H7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f>IF(H15&lt;0.32,1-((1-0.5)/0.32)*H15,(((0.5/(1-0.32))*0.32)+0.5)-(0.5/(1-0.32))*H15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="H16" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ref="I16:I25" si="1">IF(H16&lt;0.32,1-((1-0.5)/0.32)*H16,(((0.5/(1-0.32))*0.32)+0.5)-(0.5/(1-0.32))*H16)</f>
+        <v>0.84375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>0</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="H17" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B11">
+      <c r="B18">
         <v>0.32</v>
       </c>
-      <c r="C11">
+      <c r="C18">
         <v>0.2</v>
       </c>
-      <c r="D11">
+      <c r="D18">
         <v>0.05</v>
       </c>
-      <c r="E11">
+      <c r="E18">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="H18" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>0.53125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="B12">
+      <c r="B19">
         <v>0.5</v>
       </c>
-      <c r="C12">
+      <c r="C19">
         <v>0.4</v>
       </c>
-      <c r="D12">
+      <c r="D19">
         <v>0.05</v>
       </c>
-      <c r="E12">
+      <c r="E19">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="H19" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>0.44117647058823534</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>0.36764705882352944</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>0.29411764705882354</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>0.22058823529411764</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0.1470588235294118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>7.3529411764705843E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>0</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D31" t="s">
         <v>15</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B20">
+      <c r="B36">
         <v>3</v>
       </c>
-      <c r="C20">
+      <c r="C36">
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="D36">
         <v>0.5</v>
       </c>
-      <c r="E20">
+      <c r="E36">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>0</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C42" t="s">
         <v>6</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D42" t="s">
         <v>15</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E42" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>37</v>
       </c>
-      <c r="B31">
+      <c r="B47">
         <v>3</v>
       </c>
-      <c r="C31">
+      <c r="C47">
         <v>1</v>
       </c>
-      <c r="D31">
+      <c r="D47">
         <v>0.5</v>
       </c>
-      <c r="E31">
+      <c r="E47">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>42</v>
+      </c>
+      <c r="I50" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H51" s="1">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <f>IF(H51&lt;0.34,1-((1-0.5)/0.34)*H51,(((0.5/(1-0.34))*0.34)+0.5)-(0.5/(1-0.34))*H51)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="H52" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I52">
+        <f t="shared" ref="I52:I61" si="2">IF(H52&lt;0.34,1-((1-0.5)/0.34)*H52,(((0.5/(1-0.34))*0.34)+0.5)-(0.5/(1-0.34))*H52)</f>
+        <v>0.8529411764705882</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>0</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C53" t="s">
         <v>6</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D53" t="s">
         <v>15</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E53" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="H53" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="2"/>
+        <v>0.70588235294117641</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>33</v>
       </c>
-      <c r="B38">
+      <c r="B54">
         <v>0.34</v>
       </c>
-      <c r="C38">
+      <c r="C54">
         <v>0.2</v>
       </c>
-      <c r="D38">
+      <c r="D54">
         <v>0.05</v>
       </c>
-      <c r="E38">
+      <c r="E54">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="H54" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="2"/>
+        <v>0.55882352941176472</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>34</v>
       </c>
-      <c r="B39">
+      <c r="B55">
         <v>0.5</v>
       </c>
-      <c r="C39">
+      <c r="C55">
         <v>0.4</v>
       </c>
-      <c r="D39">
+      <c r="D55">
         <v>0.05</v>
       </c>
-      <c r="E39">
+      <c r="E55">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="H55" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="2"/>
+        <v>0.45454545454545447</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H56" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="2"/>
+        <v>0.37878787878787873</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H57" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="2"/>
+        <v>0.30303030303030298</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H58" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="2"/>
+        <v>0.22727272727272718</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H59" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="2"/>
+        <v>0.15151515151515138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H60" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="2"/>
+        <v>7.575757575757569E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="2"/>
+        <v>-1.1102230246251565E-16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>0</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C66" t="s">
         <v>6</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D66" t="s">
         <v>15</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E66" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>35</v>
       </c>
-      <c r="B49">
+      <c r="B67">
         <v>0.5</v>
       </c>
-      <c r="C49">
+      <c r="C67">
         <v>0.4</v>
       </c>
-      <c r="D49">
+      <c r="D67">
         <v>0.05</v>
       </c>
-      <c r="E49">
+      <c r="E67">
         <v>0.6</v>
       </c>
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H71" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Flowcharts lifestages and moving system + Model documentation for CPB
</commit_message>
<xml_diff>
--- a/docs/Randomness in code explained.xlsx
+++ b/docs/Randomness in code explained.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
   <si>
     <t>Default</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Job 4 and 5 attractiveness</t>
+  </si>
+  <si>
+    <t>Resistance to move increase through Time since moving</t>
   </si>
 </sst>
 </file>
@@ -225,6 +228,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -242,7 +246,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Resistance to Move</c:v>
+                  <c:v>Resistance to move increase through Time since moving</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -251,103 +255,105 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>RTM_TimeSinceMoving!$A$12:$A$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+            <c:strRef>
+              <c:f>RTM_TimeSinceMoving!$A$11:$A$41</c:f>
+              <c:strCache>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
+                  <c:v>TimeSinceMoving</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>30</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -458,11 +464,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="139001856"/>
-        <c:axId val="139003392"/>
+        <c:axId val="107209088"/>
+        <c:axId val="107145472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139001856"/>
+        <c:axId val="107209088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -472,12 +478,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139003392"/>
+        <c:crossAx val="107145472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139003392"/>
+        <c:axId val="107145472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,15 +494,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139001856"/>
+        <c:crossAx val="107209088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -659,11 +661,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="139052928"/>
-        <c:axId val="139054464"/>
+        <c:axId val="115591040"/>
+        <c:axId val="115592576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139052928"/>
+        <c:axId val="115591040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,12 +675,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139054464"/>
+        <c:crossAx val="115592576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139054464"/>
+        <c:axId val="115592576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -689,16 +691,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139052928"/>
+        <c:crossAx val="115591040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -846,11 +843,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133631360"/>
-        <c:axId val="133649536"/>
+        <c:axId val="123538816"/>
+        <c:axId val="123556992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133631360"/>
+        <c:axId val="123538816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -860,12 +857,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133649536"/>
+        <c:crossAx val="123556992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133649536"/>
+        <c:axId val="123556992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,16 +873,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133631360"/>
+        <c:crossAx val="123538816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1033,11 +1025,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133674112"/>
-        <c:axId val="133675648"/>
+        <c:axId val="123585664"/>
+        <c:axId val="123587200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133674112"/>
+        <c:axId val="123585664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,12 +1039,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133675648"/>
+        <c:crossAx val="123587200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133675648"/>
+        <c:axId val="123587200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1063,16 +1055,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133674112"/>
+        <c:crossAx val="123585664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1220,11 +1207,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65245568"/>
-        <c:axId val="65243776"/>
+        <c:axId val="123629952"/>
+        <c:axId val="123631488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65245568"/>
+        <c:axId val="123629952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1234,12 +1221,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65243776"/>
+        <c:crossAx val="123631488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65243776"/>
+        <c:axId val="123631488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,16 +1237,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65245568"/>
+        <c:crossAx val="123629952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1276,20 +1258,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1721,8 +1703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,7 +1846,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2147,8 +2129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,7 +2527,7 @@
         <v>0.02</v>
       </c>
       <c r="I32">
-        <f t="shared" ref="I31:I40" si="2">IF(H32&lt;0.04,1-(0.5/0.04)*H32,MIN(0.6,10*H32))</f>
+        <f t="shared" ref="I32:I40" si="2">IF(H32&lt;0.04,1-(0.5/0.04)*H32,MIN(0.6,10*H32))</f>
         <v>0.75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
initial analysis files and results
</commit_message>
<xml_diff>
--- a/docs/Randomness in code explained.xlsx
+++ b/docs/Randomness in code explained.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="27795" windowHeight="11055" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="27795" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="RTM_TimeSinceMoving" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -216,7 +216,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -464,11 +464,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="107209088"/>
-        <c:axId val="107145472"/>
+        <c:axId val="122057088"/>
+        <c:axId val="122058624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107209088"/>
+        <c:axId val="122057088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -478,12 +478,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107145472"/>
+        <c:crossAx val="122058624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107145472"/>
+        <c:axId val="122058624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +494,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107209088"/>
+        <c:crossAx val="122057088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -514,7 +514,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -661,11 +661,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115591040"/>
-        <c:axId val="115592576"/>
+        <c:axId val="122521088"/>
+        <c:axId val="122522624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115591040"/>
+        <c:axId val="122521088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -675,12 +675,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115592576"/>
+        <c:crossAx val="122522624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115592576"/>
+        <c:axId val="122522624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -691,7 +691,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115591040"/>
+        <c:crossAx val="122521088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -711,7 +711,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -843,11 +843,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123538816"/>
-        <c:axId val="123556992"/>
+        <c:axId val="123087488"/>
+        <c:axId val="123089280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123538816"/>
+        <c:axId val="123087488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -857,12 +857,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123556992"/>
+        <c:crossAx val="123089280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123556992"/>
+        <c:axId val="123089280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -873,7 +873,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123538816"/>
+        <c:crossAx val="123087488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -893,7 +893,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1025,11 +1025,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123585664"/>
-        <c:axId val="123587200"/>
+        <c:axId val="123113472"/>
+        <c:axId val="123115008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123585664"/>
+        <c:axId val="123113472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1039,12 +1039,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123587200"/>
+        <c:crossAx val="123115008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123587200"/>
+        <c:axId val="123115008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,7 +1055,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123585664"/>
+        <c:crossAx val="123113472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1075,7 +1075,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1207,11 +1207,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="123629952"/>
-        <c:axId val="123631488"/>
+        <c:axId val="123286656"/>
+        <c:axId val="123288192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="123629952"/>
+        <c:axId val="123286656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1221,12 +1221,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123631488"/>
+        <c:crossAx val="123288192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123631488"/>
+        <c:axId val="123288192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,7 +1237,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123629952"/>
+        <c:crossAx val="123286656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1415,9 +1415,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1455,7 +1455,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1527,7 +1527,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1703,8 +1703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1835,7 +1835,7 @@
         <v>0.01</v>
       </c>
       <c r="E8" s="1">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -2129,8 +2129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>